<commit_message>
Update of IT Catalog.
</commit_message>
<xml_diff>
--- a/ITCatalog.xlsx
+++ b/ITCatalog.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
     <sheet name="Vendors" sheetId="3" r:id="rId3"/>
     <sheet name="Versions" sheetId="4" r:id="rId4"/>
+    <sheet name="Licenses" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -106,13 +107,61 @@
   </si>
   <si>
     <t>Incremental Versions</t>
+  </si>
+  <si>
+    <t>vnd-oracle</t>
+  </si>
+  <si>
+    <t>vnd-microsoft</t>
+  </si>
+  <si>
+    <t>vnd-ibm</t>
+  </si>
+  <si>
+    <t>vnd-apple</t>
+  </si>
+  <si>
+    <t>vnd-apache</t>
+  </si>
+  <si>
+    <t>vnd-redhat</t>
+  </si>
+  <si>
+    <t>vnd-novell</t>
+  </si>
+  <si>
+    <t>prd-tomcat</t>
+  </si>
+  <si>
+    <t>lcs-apl2</t>
+  </si>
+  <si>
+    <t>Apache License 2.0</t>
+  </si>
+  <si>
+    <t>cat-jee-web</t>
+  </si>
+  <si>
+    <t>cat-app-server</t>
+  </si>
+  <si>
+    <t>cat-jee-app-server</t>
+  </si>
+  <si>
+    <t>cat-rdb</t>
+  </si>
+  <si>
+    <t>cat-graph-db</t>
+  </si>
+  <si>
+    <t>cat-column-store</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,13 +185,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,8 +226,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -505,7 +571,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -514,26 +580,38 @@
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
       <c r="B2" t="s">
         <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -548,34 +626,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -584,6 +666,9 @@
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -592,6 +677,9 @@
       </c>
     </row>
     <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -599,37 +687,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="B12" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -646,59 +733,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="14" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -712,33 +824,70 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="96.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>